<commit_message>
the transients has been fixed
</commit_message>
<xml_diff>
--- a/Monitor_probabilities_AUC.xlsx
+++ b/Monitor_probabilities_AUC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhysioUser\Desktop\PhD\Monitor\Codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhysioUser\OneDrive - University College Cork\Monitor\Codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E34112-F8A6-4D60-A143-6A0D3680AB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07769E8F-54F9-4B11-9C35-4B78AED27575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -44,16 +44,64 @@
     <t>AUC</t>
   </si>
   <si>
-    <t>prob_MRI (0.1_4_0.7_0_2_500)</t>
+    <t>prob_MRI_NIRS(0.05_3_0.8_0_1_500)</t>
   </si>
   <si>
-    <t>prob_MRI (0.01_4_1_1_1_100)</t>
+    <t>prob_MRI_NIRS(0.1_4_1_1_1_100)</t>
   </si>
   <si>
-    <t>prob HIE (0.05_5_0.8_0_1_50)</t>
+    <t>95% CI</t>
   </si>
   <si>
-    <t>prob HIE (0.1_4_0.9_0_1_50)</t>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Senistivity</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>prob_HIE_NIRS(0.1_6_0.8_0_1_100)</t>
+  </si>
+  <si>
+    <t>prob_HIE_NIRS(0.01_6_0.9_1_1_500)</t>
+  </si>
+  <si>
+    <t>prob_MRI (0.01_3_0.7_1_2_100)</t>
+  </si>
+  <si>
+    <t>prob_MRI (0.05_3_1_0_2_500)</t>
+  </si>
+  <si>
+    <t>prob HIE (0.1_6_0.7_0_1_100)</t>
+  </si>
+  <si>
+    <t>prob HIE (0.05_3_1_0_1_500)</t>
+  </si>
+  <si>
+    <t>0.3244    0.6560</t>
+  </si>
+  <si>
+    <t>0.3063    0.6482</t>
+  </si>
+  <si>
+    <t>0.6838    0.9110</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6577    0.8948</t>
+  </si>
+  <si>
+    <t>0.6862    0.9250</t>
+  </si>
+  <si>
+    <t>0.6866    0.9163</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5626    0.8326</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5575    0.8268</t>
   </si>
 </sst>
 </file>
@@ -69,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +136,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -101,16 +161,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -385,1060 +453,1911 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.34132380000000001</v>
+        <v>0.36124104000000001</v>
       </c>
       <c r="C2">
-        <v>0.31436302999999999</v>
+        <v>0.42445690000000003</v>
       </c>
       <c r="D2">
-        <v>0.12681709999999999</v>
+        <v>8.7431919999999996E-2</v>
       </c>
       <c r="E2">
-        <v>0.10332236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7.9053479999999995E-2</v>
+      </c>
+      <c r="F2">
+        <v>0.42749077000000002</v>
+      </c>
+      <c r="G2">
+        <v>0.43983132000000003</v>
+      </c>
+      <c r="H2">
+        <v>0.25416784999999997</v>
+      </c>
+      <c r="I2">
+        <v>0.38721614999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3.1281789E-3</v>
+        <v>0.25462045999999999</v>
       </c>
       <c r="C3">
-        <v>0.23559408000000001</v>
+        <v>8.6662270000000003E-3</v>
       </c>
       <c r="D3">
-        <v>0.56781510000000002</v>
+        <v>0.71438235000000005</v>
       </c>
       <c r="E3">
-        <v>0.5818662</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.74156575999999996</v>
+      </c>
+      <c r="F3">
+        <v>0.16751332999999999</v>
+      </c>
+      <c r="G3">
+        <v>0.18412970000000001</v>
+      </c>
+      <c r="H3">
+        <v>0.86110127000000003</v>
+      </c>
+      <c r="I3">
+        <v>0.8008478</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>8.3958720000000001E-2</v>
+        <v>0.30546820000000002</v>
       </c>
       <c r="C4">
-        <v>0.24055614</v>
+        <v>0.16188026999999999</v>
       </c>
       <c r="D4">
-        <v>0.11919188</v>
+        <v>2.0824423000000002E-2</v>
       </c>
       <c r="E4">
-        <v>4.6711057E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.3151642E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.15371029999999999</v>
+      </c>
+      <c r="G4">
+        <v>0.14107454</v>
+      </c>
+      <c r="H4">
+        <v>0.73227070000000005</v>
+      </c>
+      <c r="I4">
+        <v>0.72887829999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.43606886</v>
+        <v>0.48539465999999998</v>
       </c>
       <c r="C5">
-        <v>0.53598325999999996</v>
+        <v>0.27835503</v>
       </c>
       <c r="D5">
-        <v>0.86480140000000005</v>
+        <v>0.96367590000000003</v>
       </c>
       <c r="E5">
-        <v>0.94116264999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.96326524000000002</v>
+      </c>
+      <c r="F5">
+        <v>0.27135140000000002</v>
+      </c>
+      <c r="G5">
+        <v>0.29366704999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.89939075999999996</v>
+      </c>
+      <c r="I5">
+        <v>0.85361560000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.15408595999999999</v>
+        <v>0.38305768000000001</v>
       </c>
       <c r="C6">
-        <v>0.34461631999999998</v>
+        <v>5.7396434000000003E-2</v>
       </c>
       <c r="D6">
-        <v>0.53336879999999998</v>
+        <v>0.80226620000000004</v>
       </c>
       <c r="E6">
-        <v>0.66982819999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.80674000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.45657599999999998</v>
+      </c>
+      <c r="G6">
+        <v>0.46796796000000002</v>
+      </c>
+      <c r="H6">
+        <v>0.88210239999999995</v>
+      </c>
+      <c r="I6">
+        <v>0.84363924999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.11542921</v>
+        <v>0.32068118000000001</v>
       </c>
       <c r="C7">
-        <v>0.2452761</v>
+        <v>0.21841994000000001</v>
       </c>
       <c r="D7">
-        <v>0.80547869999999999</v>
+        <v>0.88319164999999999</v>
       </c>
       <c r="E7">
-        <v>0.90062580000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.89521295000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.16822195000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.17204875</v>
+      </c>
+      <c r="H7">
+        <v>0.84320870000000003</v>
+      </c>
+      <c r="I7">
+        <v>0.83106000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>3.4976925999999998E-2</v>
+        <v>0.30092079999999999</v>
       </c>
       <c r="C8">
-        <v>0.2452761</v>
+        <v>4.9161169999999997E-2</v>
       </c>
       <c r="D8">
-        <v>0.55141090000000004</v>
+        <v>0.54095733000000001</v>
       </c>
       <c r="E8">
-        <v>0.39852982999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.1903937</v>
+      </c>
+      <c r="F8">
+        <v>0.24721596000000001</v>
+      </c>
+      <c r="G8">
+        <v>0.26095963</v>
+      </c>
+      <c r="H8">
+        <v>0.84004027000000003</v>
+      </c>
+      <c r="I8">
+        <v>0.79904889999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1.0230804E-2</v>
+        <v>0.26559460000000001</v>
       </c>
       <c r="C9">
-        <v>0.24077933000000001</v>
+        <v>1.9443812000000001E-2</v>
       </c>
       <c r="D9">
-        <v>0.47265406999999998</v>
+        <v>0.46109783999999998</v>
       </c>
       <c r="E9">
-        <v>0.56703400000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.54205729999999996</v>
+      </c>
+      <c r="F9">
+        <v>0.22281024999999999</v>
+      </c>
+      <c r="G9">
+        <v>0.23286390000000001</v>
+      </c>
+      <c r="H9">
+        <v>0.95212764000000005</v>
+      </c>
+      <c r="I9">
+        <v>0.88984525000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>5.3336800000000004E-3</v>
+        <v>0.27814060000000002</v>
       </c>
       <c r="C10">
-        <v>0.24027693</v>
+        <v>1.5667154999999999E-2</v>
       </c>
       <c r="D10">
-        <v>0.22710279999999999</v>
+        <v>0.39147567999999999</v>
       </c>
       <c r="E10">
-        <v>0.30507582</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.46754279999999998</v>
+      </c>
+      <c r="F10">
+        <v>0.13343446</v>
+      </c>
+      <c r="G10">
+        <v>0.15642186</v>
+      </c>
+      <c r="H10">
+        <v>0.60213846000000004</v>
+      </c>
+      <c r="I10">
+        <v>0.63277600000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4.4044560000000003E-2</v>
+        <v>0.37853540000000002</v>
       </c>
       <c r="C11">
-        <v>0.46127321999999998</v>
+        <v>7.7594854000000005E-2</v>
       </c>
       <c r="D11">
-        <v>0.56058127000000002</v>
+        <v>0.51438269999999997</v>
       </c>
       <c r="E11">
-        <v>0.60521084000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.5094379</v>
+      </c>
+      <c r="F11">
+        <v>0.69930740000000002</v>
+      </c>
+      <c r="G11">
+        <v>0.65946364000000002</v>
+      </c>
+      <c r="H11">
+        <v>0.92342639999999998</v>
+      </c>
+      <c r="I11">
+        <v>0.86115920000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>7.2890944999999999E-2</v>
+        <v>0.30291304000000002</v>
       </c>
       <c r="C12">
-        <v>0.25030683999999997</v>
+        <v>8.9750945999999998E-2</v>
       </c>
       <c r="D12">
-        <v>0.78301900000000002</v>
+        <v>0.94905673999999995</v>
       </c>
       <c r="E12">
-        <v>0.91172534000000005</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.93244119999999997</v>
+      </c>
+      <c r="F12">
+        <v>0.29420170000000001</v>
+      </c>
+      <c r="G12">
+        <v>0.29341060000000002</v>
+      </c>
+      <c r="H12">
+        <v>0.74001620000000001</v>
+      </c>
+      <c r="I12">
+        <v>0.70975699999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.808867</v>
+        <v>0.55314189999999996</v>
       </c>
       <c r="C13">
-        <v>0.54977589999999998</v>
+        <v>0.57760054000000005</v>
       </c>
       <c r="D13">
-        <v>0.83073520000000001</v>
+        <v>0.88601260000000004</v>
       </c>
       <c r="E13">
-        <v>0.86926853999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.93581985999999995</v>
+      </c>
+      <c r="F13">
+        <v>0.35419148</v>
+      </c>
+      <c r="G13">
+        <v>0.32999395999999998</v>
+      </c>
+      <c r="H13">
+        <v>0.80059515999999997</v>
+      </c>
+      <c r="I13">
+        <v>0.77247672999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.42583427000000001</v>
+        <v>0.45173471999999998</v>
       </c>
       <c r="C14">
-        <v>0.32314894</v>
+        <v>0.39920127</v>
       </c>
       <c r="D14">
-        <v>0.25508599999999998</v>
+        <v>7.8797300000000001E-2</v>
       </c>
       <c r="E14">
-        <v>0.21254458000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.4676800000000003E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.10013384</v>
+      </c>
+      <c r="G14">
+        <v>0.102688245</v>
+      </c>
+      <c r="H14">
+        <v>0.64067629999999998</v>
+      </c>
+      <c r="I14">
+        <v>0.6344284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>15</v>
       </c>
       <c r="B15">
-        <v>6.1161607999999999E-2</v>
+        <v>0.28619625999999998</v>
       </c>
       <c r="C15">
-        <v>0.23058334</v>
+        <v>0.16784673999999999</v>
       </c>
       <c r="D15">
-        <v>0.85666419999999999</v>
+        <v>0.88441013999999996</v>
       </c>
       <c r="E15">
-        <v>0.88785314999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.84399650000000004</v>
+      </c>
+      <c r="F15">
+        <v>0.34567155999999999</v>
+      </c>
+      <c r="G15">
+        <v>0.34708329999999998</v>
+      </c>
+      <c r="H15">
+        <v>0.97510319999999995</v>
+      </c>
+      <c r="I15">
+        <v>0.94743230000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.23689117000000001</v>
+        <v>0.3421825</v>
       </c>
       <c r="C16">
-        <v>0.28398006999999997</v>
+        <v>4.1238802999999997E-2</v>
       </c>
       <c r="D16">
-        <v>0.22065997000000001</v>
+        <v>5.8875381999999997E-2</v>
       </c>
       <c r="E16">
-        <v>0.14968998999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6.3352494999999995E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.25342724</v>
+      </c>
+      <c r="G16">
+        <v>0.26766032000000001</v>
+      </c>
+      <c r="H16">
+        <v>0.71108024999999997</v>
+      </c>
+      <c r="I16">
+        <v>0.66923379999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.28996706</v>
+        <v>0.32459779999999999</v>
       </c>
       <c r="C17">
-        <v>0.27172383999999999</v>
+        <v>0.52005654999999995</v>
       </c>
       <c r="D17">
-        <v>0.74411660000000002</v>
+        <v>0.63948196000000002</v>
       </c>
       <c r="E17">
-        <v>0.69063985000000006</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.5869143</v>
+      </c>
+      <c r="F17">
+        <v>0.22338348999999999</v>
+      </c>
+      <c r="G17">
+        <v>0.23498348999999999</v>
+      </c>
+      <c r="H17">
+        <v>0.84504760000000001</v>
+      </c>
+      <c r="I17">
+        <v>0.8175962</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.84240919999999997</v>
+        <v>0.49577346</v>
       </c>
       <c r="C18">
-        <v>0.32375029999999999</v>
+        <v>0.72466540000000002</v>
       </c>
       <c r="D18">
-        <v>0.84755959999999997</v>
+        <v>0.85011274000000003</v>
       </c>
       <c r="E18">
-        <v>0.87326000000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.90131413999999999</v>
+      </c>
+      <c r="F18">
+        <v>0.27870430000000002</v>
+      </c>
+      <c r="G18">
+        <v>0.29256406000000001</v>
+      </c>
+      <c r="H18">
+        <v>0.91062343000000001</v>
+      </c>
+      <c r="I18">
+        <v>0.8703864</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.31154494999999999</v>
+        <v>0.39467405999999999</v>
       </c>
       <c r="C19">
-        <v>0.41405436000000001</v>
+        <v>0.4442391</v>
       </c>
       <c r="D19">
-        <v>0.7167713</v>
+        <v>0.47471385999999999</v>
       </c>
       <c r="E19">
-        <v>0.83051585999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.77096869999999995</v>
+      </c>
+      <c r="F19">
+        <v>0.25446266000000001</v>
+      </c>
+      <c r="G19">
+        <v>0.24482292999999999</v>
+      </c>
+      <c r="H19">
+        <v>0.48771485999999997</v>
+      </c>
+      <c r="I19">
+        <v>0.48483542000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.80995846000000005</v>
+        <v>0.59341310000000003</v>
       </c>
       <c r="C20">
-        <v>0.56893579999999999</v>
+        <v>0.80117923000000002</v>
       </c>
       <c r="D20">
-        <v>0.83786419999999995</v>
+        <v>0.87491569999999996</v>
       </c>
       <c r="E20">
-        <v>0.91661789999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.92321472999999998</v>
+      </c>
+      <c r="F20">
+        <v>0.24714747000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.23856598000000001</v>
+      </c>
+      <c r="H20">
+        <v>0.86708070000000004</v>
+      </c>
+      <c r="I20">
+        <v>0.82192770000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>21</v>
       </c>
       <c r="B21">
-        <v>0.30656033999999999</v>
+        <v>0.33671610000000002</v>
       </c>
       <c r="C21">
-        <v>0.38747817000000001</v>
+        <v>0.27827433000000001</v>
       </c>
       <c r="D21">
-        <v>0.62406459999999997</v>
+        <v>0.30081596999999999</v>
       </c>
       <c r="E21">
-        <v>0.44040045</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.22326170000000001</v>
+      </c>
+      <c r="F21">
+        <v>0.34494155999999998</v>
+      </c>
+      <c r="G21">
+        <v>0.35826337000000003</v>
+      </c>
+      <c r="H21">
+        <v>0.3940922</v>
+      </c>
+      <c r="I21">
+        <v>0.41962945000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0.34529506999999998</v>
+        <v>0.52434510000000001</v>
       </c>
       <c r="C22">
-        <v>0.53200899999999995</v>
+        <v>0.34775233</v>
       </c>
       <c r="D22">
-        <v>0.75557660000000004</v>
+        <v>0.90329519999999996</v>
       </c>
       <c r="E22">
-        <v>0.86576235000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.93003975999999999</v>
+      </c>
+      <c r="F22">
+        <v>0.52597830000000001</v>
+      </c>
+      <c r="G22">
+        <v>0.50403070000000005</v>
+      </c>
+      <c r="H22">
+        <v>0.98689389999999999</v>
+      </c>
+      <c r="I22">
+        <v>0.96434330000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>23</v>
       </c>
       <c r="B23">
-        <v>2.3427534999999999E-2</v>
+        <v>0.30667361999999998</v>
       </c>
       <c r="C23">
-        <v>0.26906945999999998</v>
+        <v>5.5379860000000003E-2</v>
       </c>
       <c r="D23">
-        <v>0.13911477</v>
+        <v>6.2676979999999993E-2</v>
       </c>
       <c r="E23">
-        <v>8.1279710000000005E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6.5595970000000003E-2</v>
+      </c>
+      <c r="F23">
+        <v>0.36442170000000002</v>
+      </c>
+      <c r="G23">
+        <v>0.37779439999999997</v>
+      </c>
+      <c r="H23">
+        <v>0.51095239999999997</v>
+      </c>
+      <c r="I23">
+        <v>0.50869876000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.48842819999999998</v>
+        <v>0.38900976999999998</v>
       </c>
       <c r="C24">
-        <v>0.48904234000000002</v>
+        <v>0.59808165000000002</v>
       </c>
       <c r="D24">
-        <v>0.90361599999999997</v>
+        <v>0.98837763000000001</v>
       </c>
       <c r="E24">
-        <v>0.97006049999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.99424356000000003</v>
+      </c>
+      <c r="F24">
+        <v>0.27678355999999998</v>
+      </c>
+      <c r="G24">
+        <v>0.26921919999999999</v>
+      </c>
+      <c r="H24">
+        <v>0.79562854999999999</v>
+      </c>
+      <c r="I24">
+        <v>0.78555447</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>25</v>
       </c>
       <c r="B25">
-        <v>9.2270199999999997E-2</v>
+        <v>0.26509386000000001</v>
       </c>
       <c r="C25">
-        <v>0.27076425999999998</v>
+        <v>0.11586812</v>
       </c>
       <c r="D25">
-        <v>0.46332413</v>
+        <v>0.31363669999999999</v>
       </c>
       <c r="E25">
-        <v>0.48168135000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.51556844000000002</v>
+      </c>
+      <c r="F25">
+        <v>0.25283757000000001</v>
+      </c>
+      <c r="G25">
+        <v>0.25134727000000001</v>
+      </c>
+      <c r="H25">
+        <v>0.86775930000000001</v>
+      </c>
+      <c r="I25">
+        <v>0.85637319999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>26</v>
       </c>
       <c r="B26">
-        <v>5.5195639999999997E-2</v>
+        <v>0.30881658000000001</v>
       </c>
       <c r="C26">
-        <v>0.38022178000000001</v>
+        <v>9.1687939999999996E-2</v>
       </c>
       <c r="D26">
-        <v>0.84732264000000002</v>
+        <v>0.90634400000000004</v>
       </c>
       <c r="E26">
-        <v>0.89305159999999995</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.88117160000000005</v>
+      </c>
+      <c r="F26">
+        <v>0.38774118000000002</v>
+      </c>
+      <c r="G26">
+        <v>0.33602956</v>
+      </c>
+      <c r="H26">
+        <v>0.71649843000000002</v>
+      </c>
+      <c r="I26">
+        <v>0.69184080000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0.44016522000000002</v>
+        <v>0.61882800000000004</v>
       </c>
       <c r="C27">
-        <v>0.68499993999999997</v>
+        <v>0.814052</v>
       </c>
       <c r="D27">
-        <v>0.76918620000000004</v>
+        <v>0.68742060000000005</v>
       </c>
       <c r="E27">
-        <v>0.72304630000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.60810470000000005</v>
+      </c>
+      <c r="F27">
+        <v>0.26847850000000001</v>
+      </c>
+      <c r="G27">
+        <v>0.28553793</v>
+      </c>
+      <c r="H27">
+        <v>0.78030679999999997</v>
+      </c>
+      <c r="I27">
+        <v>0.73226440000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>28</v>
       </c>
       <c r="B28">
-        <v>0.95627609999999996</v>
+        <v>0.63083195999999997</v>
       </c>
       <c r="C28">
-        <v>0.68527764000000002</v>
+        <v>0.88426804999999997</v>
       </c>
       <c r="D28">
-        <v>0.90926874000000002</v>
+        <v>0.98613629999999997</v>
       </c>
       <c r="E28">
-        <v>0.96195120000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.99302024</v>
+      </c>
+      <c r="F28">
+        <v>0.27273409999999998</v>
+      </c>
+      <c r="G28">
+        <v>0.31000042</v>
+      </c>
+      <c r="H28">
+        <v>0.89066889999999999</v>
+      </c>
+      <c r="I28">
+        <v>0.86021537000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0.37568562999999999</v>
+        <v>0.34665963</v>
       </c>
       <c r="C29">
-        <v>0.41346884</v>
+        <v>0.25447127000000003</v>
       </c>
       <c r="D29">
-        <v>0.85636955000000003</v>
+        <v>0.86918664000000001</v>
       </c>
       <c r="E29">
-        <v>0.73850229999999994</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+        <v>0.8472191</v>
+      </c>
+      <c r="F29">
+        <v>0.31062397000000003</v>
+      </c>
+      <c r="G29">
+        <v>0.29671258</v>
+      </c>
+      <c r="H29">
+        <v>0.86280864000000002</v>
+      </c>
+      <c r="I29">
+        <v>0.84809493999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
         <v>30</v>
       </c>
-      <c r="D30">
-        <v>0.35939860000000001</v>
-      </c>
-      <c r="E30">
-        <v>0.3949281</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="3">
+        <v>0.61840326000000001</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.70046025999999995</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0.82013499999999995</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0.76636212999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>31</v>
       </c>
-      <c r="B31">
-        <v>0.10337515999999999</v>
-      </c>
-      <c r="C31">
-        <v>0.27269297999999997</v>
+      <c r="B31" s="4">
+        <v>0.34491949999999999</v>
+      </c>
+      <c r="C31" s="4">
+        <v>8.6517960000000005E-2</v>
       </c>
       <c r="D31">
-        <v>0.47089915999999998</v>
+        <v>0.76419084999999998</v>
       </c>
       <c r="E31">
-        <v>0.61949929999999997</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.7418479</v>
+      </c>
+      <c r="F31">
+        <v>0.27317718000000002</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0.26681936000000001</v>
+      </c>
+      <c r="H31">
+        <v>0.75137880000000001</v>
+      </c>
+      <c r="I31">
+        <v>0.72701733999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>32</v>
       </c>
       <c r="B32">
-        <v>0.83101930000000002</v>
+        <v>0.55250290000000002</v>
       </c>
       <c r="C32">
-        <v>0.57039819999999997</v>
+        <v>0.81152159999999995</v>
       </c>
       <c r="D32">
-        <v>0.13003524</v>
+        <v>6.7204386000000005E-2</v>
       </c>
       <c r="E32">
-        <v>7.3743710000000004E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.0880477E-2</v>
+      </c>
+      <c r="F32">
+        <v>0.52016779999999996</v>
+      </c>
+      <c r="G32">
+        <v>0.46568638000000001</v>
+      </c>
+      <c r="H32">
+        <v>0.24457868999999999</v>
+      </c>
+      <c r="I32">
+        <v>0.28809847999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>33</v>
       </c>
       <c r="B33">
-        <v>0.19324362</v>
+        <v>0.3857584</v>
       </c>
       <c r="C33">
-        <v>0.42779993999999999</v>
+        <v>0.28736191999999999</v>
       </c>
       <c r="D33">
-        <v>0.3879822</v>
+        <v>0.64288294000000001</v>
       </c>
       <c r="E33">
-        <v>0.43414760000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.84379183999999996</v>
+      </c>
+      <c r="F33">
+        <v>0.24779087</v>
+      </c>
+      <c r="G33">
+        <v>0.23199230000000001</v>
+      </c>
+      <c r="H33">
+        <v>0.89297110000000002</v>
+      </c>
+      <c r="I33">
+        <v>0.86587040000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>34</v>
       </c>
       <c r="B34">
-        <v>3.7233761999999997E-2</v>
+        <v>0.30234149999999999</v>
       </c>
       <c r="C34">
-        <v>0.30259796999999999</v>
+        <v>7.0744429999999997E-2</v>
       </c>
       <c r="D34">
-        <v>0.10769846</v>
+        <v>1.9057902000000002E-2</v>
       </c>
       <c r="E34">
-        <v>4.9218150000000002E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.8166603999999999E-2</v>
+      </c>
+      <c r="F34">
+        <v>4.5782976000000003E-2</v>
+      </c>
+      <c r="G34">
+        <v>5.4567686999999997E-2</v>
+      </c>
+      <c r="H34">
+        <v>0.75057185000000004</v>
+      </c>
+      <c r="I34">
+        <v>0.72097254</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>35</v>
       </c>
       <c r="B35">
-        <v>0.12363869</v>
+        <v>0.32413315999999998</v>
       </c>
       <c r="C35">
-        <v>0.40198250000000002</v>
+        <v>0.15548496000000001</v>
       </c>
       <c r="D35">
-        <v>0.53015330000000005</v>
+        <v>0.63126766999999995</v>
       </c>
       <c r="E35">
-        <v>0.62728720000000004</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.53030719999999998</v>
+      </c>
+      <c r="F35">
+        <v>0.27441555000000001</v>
+      </c>
+      <c r="G35">
+        <v>0.25244796000000003</v>
+      </c>
+      <c r="H35">
+        <v>0.76395630000000003</v>
+      </c>
+      <c r="I35">
+        <v>0.75323890000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>36</v>
       </c>
       <c r="B36">
-        <v>0.71087250000000002</v>
+        <v>0.47162983000000003</v>
       </c>
       <c r="C36">
-        <v>0.42191794999999999</v>
+        <v>0.77339380000000002</v>
       </c>
       <c r="D36">
-        <v>9.5322749999999998E-2</v>
+        <v>1.7780523999999999E-2</v>
       </c>
       <c r="E36">
-        <v>5.2682596999999998E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0325437999999999E-2</v>
+      </c>
+      <c r="F36">
+        <v>0.37988734000000002</v>
+      </c>
+      <c r="G36">
+        <v>0.40995207</v>
+      </c>
+      <c r="H36">
+        <v>0.64078089999999999</v>
+      </c>
+      <c r="I36">
+        <v>0.63990619999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>37</v>
       </c>
       <c r="B37">
-        <v>4.2026013000000001E-2</v>
+        <v>0.39545023000000001</v>
       </c>
       <c r="C37">
-        <v>0.27269297999999997</v>
+        <v>0.10702296</v>
       </c>
       <c r="D37">
-        <v>0.47785430000000001</v>
+        <v>0.23669635999999999</v>
       </c>
       <c r="E37">
-        <v>0.44946884999999998</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.30919743</v>
+      </c>
+      <c r="F37">
+        <v>0.27135223000000003</v>
+      </c>
+      <c r="G37">
+        <v>0.28695804000000003</v>
+      </c>
+      <c r="H37">
+        <v>0.91614130000000005</v>
+      </c>
+      <c r="I37">
+        <v>0.88741630000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>38</v>
       </c>
       <c r="B38">
-        <v>2.19443E-2</v>
+        <v>0.37677217000000002</v>
       </c>
       <c r="C38">
-        <v>0.35110112999999998</v>
+        <v>0.15295406</v>
       </c>
       <c r="D38">
-        <v>0.44245282000000002</v>
+        <v>0.49482991999999998</v>
       </c>
       <c r="E38">
-        <v>0.4560012</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.44480302999999999</v>
+      </c>
+      <c r="F38">
+        <v>0.50634617000000004</v>
+      </c>
+      <c r="G38">
+        <v>0.4714834</v>
+      </c>
+      <c r="H38">
+        <v>0.94346649999999999</v>
+      </c>
+      <c r="I38">
+        <v>0.90541419999999995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>39</v>
       </c>
       <c r="B39">
-        <v>0.65663559999999999</v>
+        <v>0.52067565999999998</v>
       </c>
       <c r="C39">
-        <v>0.54211503000000005</v>
+        <v>0.64132520000000004</v>
       </c>
       <c r="D39">
-        <v>0.122001834</v>
+        <v>2.9517919E-2</v>
       </c>
       <c r="E39">
-        <v>4.7449940000000003E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.3511553000000001E-2</v>
+      </c>
+      <c r="F39">
+        <v>0.54745876999999998</v>
+      </c>
+      <c r="G39">
+        <v>0.49672812</v>
+      </c>
+      <c r="H39">
+        <v>0.50128170000000005</v>
+      </c>
+      <c r="I39">
+        <v>0.47561367999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>40</v>
       </c>
       <c r="B40">
-        <v>0.27945399999999998</v>
+        <v>0.48029336</v>
       </c>
       <c r="C40">
-        <v>0.5396765</v>
+        <v>0.17538614999999999</v>
       </c>
       <c r="D40">
-        <v>0.69889210000000002</v>
+        <v>0.77763570000000004</v>
       </c>
       <c r="E40">
-        <v>0.73749200000000004</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+        <v>0.63501763</v>
+      </c>
+      <c r="F40">
+        <v>0.33067770000000002</v>
+      </c>
+      <c r="G40">
+        <v>0.34653082000000002</v>
+      </c>
+      <c r="H40">
+        <v>0.61872523999999995</v>
+      </c>
+      <c r="I40">
+        <v>0.62001220000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
         <v>41</v>
       </c>
-      <c r="D41">
-        <v>0.68097479999999999</v>
-      </c>
-      <c r="E41">
-        <v>0.75579386999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="3">
+        <v>0.95302480000000001</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.99120306999999996</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0.86435280000000003</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0.84273577</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42</v>
       </c>
       <c r="B42">
-        <v>8.7402320000000006E-2</v>
+        <v>0.28066461999999998</v>
       </c>
       <c r="C42">
-        <v>0.25329239999999997</v>
+        <v>0.24264993000000001</v>
       </c>
       <c r="D42">
-        <v>9.4866889999999995E-2</v>
+        <v>1.1803633500000001E-2</v>
       </c>
       <c r="E42">
-        <v>3.0390488E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6.2182065999999998E-3</v>
+      </c>
+      <c r="F42">
+        <v>0.19907743999999999</v>
+      </c>
+      <c r="G42">
+        <v>0.1949504</v>
+      </c>
+      <c r="H42">
+        <v>0.74207730000000005</v>
+      </c>
+      <c r="I42">
+        <v>0.71717370000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43</v>
       </c>
-      <c r="B43">
-        <v>1.4434265999999999E-2</v>
-      </c>
-      <c r="C43">
-        <v>0.31003459999999999</v>
+      <c r="B43" s="4">
+        <v>0.34063710000000003</v>
+      </c>
+      <c r="C43" s="4">
+        <v>5.7389226000000002E-2</v>
       </c>
       <c r="D43">
-        <v>0.46118882</v>
+        <v>0.27162315999999997</v>
       </c>
       <c r="E43">
-        <v>0.44672114000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.22121821</v>
+      </c>
+      <c r="F43">
+        <v>0.19279647</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0.18487653000000001</v>
+      </c>
+      <c r="H43">
+        <v>0.98030572999999999</v>
+      </c>
+      <c r="I43">
+        <v>0.95084250000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44</v>
       </c>
       <c r="B44">
-        <v>0.18706132</v>
+        <v>0.32269389999999998</v>
       </c>
       <c r="C44">
-        <v>0.37515505999999998</v>
+        <v>0.22715753</v>
       </c>
       <c r="D44">
-        <v>0.59419679999999997</v>
+        <v>0.29215289999999999</v>
       </c>
       <c r="E44">
-        <v>0.79294425000000002</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.18055837999999999</v>
+      </c>
+      <c r="F44">
+        <v>0.41924027000000003</v>
+      </c>
+      <c r="G44">
+        <v>0.42761107999999998</v>
+      </c>
+      <c r="H44">
+        <v>0.9764794</v>
+      </c>
+      <c r="I44">
+        <v>0.96310359999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45</v>
       </c>
       <c r="B45">
-        <v>0.33589859999999999</v>
+        <v>0.33045950000000002</v>
       </c>
       <c r="C45">
-        <v>0.31742749999999997</v>
+        <v>0.42817008000000001</v>
       </c>
       <c r="D45">
-        <v>8.2508973999999999E-2</v>
+        <v>1.5870929999999998E-2</v>
       </c>
       <c r="E45">
-        <v>2.8690396E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9.336235E-3</v>
+      </c>
+      <c r="F45">
+        <v>0.46368954000000001</v>
+      </c>
+      <c r="G45">
+        <v>0.48500409999999999</v>
+      </c>
+      <c r="H45">
+        <v>0.51345949999999996</v>
+      </c>
+      <c r="I45">
+        <v>0.47196270000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>46</v>
       </c>
       <c r="B46">
-        <v>0.12821189999999999</v>
+        <v>0.30030137000000001</v>
       </c>
       <c r="C46">
-        <v>0.28198810000000002</v>
+        <v>0.10017832</v>
       </c>
       <c r="D46">
-        <v>0.23314040999999999</v>
+        <v>0.29520659999999999</v>
       </c>
       <c r="E46">
-        <v>0.20542829000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.31006956000000002</v>
+      </c>
+      <c r="F46">
+        <v>0.21341599999999999</v>
+      </c>
+      <c r="G46">
+        <v>0.22137491000000001</v>
+      </c>
+      <c r="H46">
+        <v>0.86846405000000004</v>
+      </c>
+      <c r="I46">
+        <v>0.85375356999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>47</v>
       </c>
       <c r="B47">
-        <v>2.5180276000000001E-2</v>
+        <v>0.24716452999999999</v>
       </c>
       <c r="C47">
-        <v>0.24594149000000001</v>
+        <v>3.3767827E-2</v>
       </c>
       <c r="D47">
-        <v>0.23851312999999999</v>
+        <v>4.3809465999999998E-2</v>
       </c>
       <c r="E47">
-        <v>0.11295347</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.6869301E-2</v>
+      </c>
+      <c r="F47">
+        <v>0.44553965000000001</v>
+      </c>
+      <c r="G47">
+        <v>0.48800100000000002</v>
+      </c>
+      <c r="H47">
+        <v>0.76264244000000003</v>
+      </c>
+      <c r="I47">
+        <v>0.69133659999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>48</v>
       </c>
       <c r="B48">
-        <v>4.5679974999999998E-2</v>
+        <v>0.35064267999999998</v>
       </c>
       <c r="C48">
-        <v>0.29025630000000002</v>
+        <v>0.17170738999999999</v>
       </c>
       <c r="D48">
-        <v>9.4472095000000006E-2</v>
+        <v>2.4818672E-2</v>
       </c>
       <c r="E48">
-        <v>3.9013989999999998E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.5919011E-2</v>
+      </c>
+      <c r="F48">
+        <v>0.30796897000000001</v>
+      </c>
+      <c r="G48">
+        <v>0.31351075</v>
+      </c>
+      <c r="H48">
+        <v>0.20555237000000001</v>
+      </c>
+      <c r="I48">
+        <v>0.26168730000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>49</v>
       </c>
       <c r="B49">
-        <v>0.66885620000000001</v>
+        <v>0.41026395999999998</v>
       </c>
       <c r="C49">
-        <v>0.30887985000000001</v>
+        <v>0.77060925999999996</v>
       </c>
       <c r="D49">
-        <v>8.4621500000000002E-2</v>
+        <v>1.098475E-2</v>
       </c>
       <c r="E49">
-        <v>3.3422314000000002E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.32442545E-2</v>
+      </c>
+      <c r="F49">
+        <v>0.40953640000000002</v>
+      </c>
+      <c r="G49">
+        <v>0.42943153000000001</v>
+      </c>
+      <c r="H49">
+        <v>0.40600544</v>
+      </c>
+      <c r="I49">
+        <v>0.41837447999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>50</v>
       </c>
       <c r="B50">
-        <v>3.016688E-2</v>
+        <v>0.26509386000000001</v>
       </c>
       <c r="C50">
-        <v>0.39596903</v>
+        <v>3.9358404E-2</v>
       </c>
       <c r="D50">
-        <v>0.42257345000000002</v>
+        <v>0.20135196999999999</v>
       </c>
       <c r="E50">
-        <v>0.32496753</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.15643774999999999</v>
+      </c>
+      <c r="F50">
+        <v>0.21442517999999999</v>
+      </c>
+      <c r="G50">
+        <v>0.23314013</v>
+      </c>
+      <c r="H50">
+        <v>0.70683247000000005</v>
+      </c>
+      <c r="I50">
+        <v>0.6756006</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>51</v>
       </c>
       <c r="B51">
-        <v>0.45674545</v>
+        <v>0.26595950000000002</v>
       </c>
       <c r="C51">
-        <v>0.24594149000000001</v>
+        <v>0.18335731</v>
       </c>
       <c r="D51">
-        <v>0.28258643</v>
+        <v>0.20216943000000001</v>
       </c>
       <c r="E51">
-        <v>0.22198032000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.21760583999999999</v>
+      </c>
+      <c r="F51">
+        <v>0.30346960000000001</v>
+      </c>
+      <c r="G51">
+        <v>0.32264587</v>
+      </c>
+      <c r="H51">
+        <v>0.39209473</v>
+      </c>
+      <c r="I51">
+        <v>0.41156787</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>53</v>
       </c>
       <c r="B52">
-        <v>0.66725314000000002</v>
+        <v>0.63876330000000003</v>
       </c>
       <c r="C52">
-        <v>0.68148947000000004</v>
+        <v>0.67141324000000002</v>
       </c>
       <c r="D52">
-        <v>0.83036869999999996</v>
+        <v>0.97896459999999996</v>
       </c>
       <c r="E52">
-        <v>0.94245679999999998</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.99233585999999996</v>
+      </c>
+      <c r="F52">
+        <v>0.69289750000000006</v>
+      </c>
+      <c r="G52">
+        <v>0.67047540000000005</v>
+      </c>
+      <c r="H52">
+        <v>0.92617106000000005</v>
+      </c>
+      <c r="I52">
+        <v>0.91454804000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>54</v>
       </c>
       <c r="B53">
-        <v>0.95238540000000005</v>
+        <v>0.41885240000000001</v>
       </c>
       <c r="C53">
-        <v>0.44089293000000002</v>
+        <v>0.94085649999999998</v>
       </c>
       <c r="D53">
-        <v>0.10665138</v>
+        <v>3.3695704999999999E-2</v>
       </c>
       <c r="E53">
-        <v>5.659906E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.7175629999999999E-2</v>
+      </c>
+      <c r="F53">
+        <v>0.32005850000000002</v>
+      </c>
+      <c r="G53">
+        <v>0.30253667000000001</v>
+      </c>
+      <c r="H53">
+        <v>0.35544120000000001</v>
+      </c>
+      <c r="I53">
+        <v>0.4123655</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>55</v>
       </c>
       <c r="B54">
-        <v>2.2245451999999999E-2</v>
+        <v>0.29238054000000002</v>
       </c>
       <c r="C54">
-        <v>0.24077933000000001</v>
+        <v>1.8870308999999998E-2</v>
       </c>
       <c r="D54">
-        <v>0.30155477000000003</v>
+        <v>0.34465635</v>
       </c>
       <c r="E54">
-        <v>0.28415816999999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.40329883</v>
+      </c>
+      <c r="F54">
+        <v>0.36829865000000001</v>
+      </c>
+      <c r="G54">
+        <v>0.35203812000000001</v>
+      </c>
+      <c r="H54">
+        <v>0.51214170000000003</v>
+      </c>
+      <c r="I54">
+        <v>0.49898413000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>56</v>
       </c>
       <c r="B55">
-        <v>7.7906005E-2</v>
+        <v>0.50921685000000005</v>
       </c>
       <c r="C55">
-        <v>0.45882260000000002</v>
+        <v>7.9023709999999997E-2</v>
       </c>
       <c r="D55">
-        <v>0.88283129999999999</v>
+        <v>0.95516526999999996</v>
       </c>
       <c r="E55">
-        <v>0.94899743999999997</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.97191050000000001</v>
+      </c>
+      <c r="F55">
+        <v>0.29198962000000001</v>
+      </c>
+      <c r="G55">
+        <v>0.29245493</v>
+      </c>
+      <c r="H55">
+        <v>0.95978450000000004</v>
+      </c>
+      <c r="I55">
+        <v>0.93253070000000005</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>57</v>
       </c>
       <c r="B56">
-        <v>0.11268887</v>
+        <v>0.34746695</v>
       </c>
       <c r="C56">
-        <v>0.30603590000000003</v>
+        <v>0.16374918999999999</v>
       </c>
       <c r="D56">
-        <v>0.72760009999999997</v>
+        <v>0.74240170000000005</v>
       </c>
       <c r="E56">
-        <v>0.81495340000000005</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.78510809999999998</v>
+      </c>
+      <c r="F56">
+        <v>0.15138367999999999</v>
+      </c>
+      <c r="G56">
+        <v>0.17777722000000001</v>
+      </c>
+      <c r="H56">
+        <v>0.61705714</v>
+      </c>
+      <c r="I56">
+        <v>0.60051363999999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>58</v>
       </c>
       <c r="B57">
-        <v>0.86948789999999998</v>
+        <v>0.53441446999999997</v>
       </c>
       <c r="C57">
-        <v>0.56481329999999996</v>
+        <v>0.83502644000000004</v>
       </c>
       <c r="D57">
-        <v>0.88994090000000003</v>
+        <v>0.98566717000000004</v>
       </c>
       <c r="E57">
-        <v>0.95275560000000004</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.99177599999999999</v>
+      </c>
+      <c r="F57">
+        <v>0.26606693999999997</v>
+      </c>
+      <c r="G57">
+        <v>0.29222468000000001</v>
+      </c>
+      <c r="H57">
+        <v>0.90967387</v>
+      </c>
+      <c r="I57">
+        <v>0.87688449999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>59</v>
       </c>
       <c r="B58">
-        <v>0.62996700000000005</v>
+        <v>0.37208095000000002</v>
       </c>
       <c r="C58">
-        <v>0.34648469999999998</v>
+        <v>0.63931537000000005</v>
       </c>
       <c r="D58">
-        <v>0.29440737</v>
+        <v>0.10561361</v>
       </c>
       <c r="E58">
-        <v>0.16238385</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8.8548199999999994E-2</v>
+      </c>
+      <c r="F58">
+        <v>0.31733567000000001</v>
+      </c>
+      <c r="G58">
+        <v>0.34508549999999999</v>
+      </c>
+      <c r="H58">
+        <v>0.47220123000000003</v>
+      </c>
+      <c r="I58">
+        <v>0.48654969999999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>60</v>
       </c>
       <c r="B59">
-        <v>1.0717590000000001E-2</v>
+        <v>0.26559460000000001</v>
       </c>
       <c r="C59">
-        <v>0.25715803999999998</v>
+        <v>1.9443812000000001E-2</v>
       </c>
       <c r="D59">
-        <v>0.26275530000000002</v>
+        <v>0.22690557</v>
       </c>
       <c r="E59">
-        <v>0.24508509000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.22518186000000001</v>
+      </c>
+      <c r="F59">
+        <v>0.16171362</v>
+      </c>
+      <c r="G59">
+        <v>0.18947758000000001</v>
+      </c>
+      <c r="H59">
+        <v>0.90794520000000001</v>
+      </c>
+      <c r="I59">
+        <v>0.858074</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>61</v>
       </c>
       <c r="B60">
-        <v>6.5707710000000003E-2</v>
+        <v>0.51482660000000002</v>
       </c>
       <c r="C60">
-        <v>0.37131008999999998</v>
+        <v>0.2876358</v>
       </c>
       <c r="D60">
-        <v>0.45793125000000001</v>
+        <v>0.26016536000000001</v>
       </c>
       <c r="E60">
-        <v>0.29311480000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.21819720000000001</v>
+      </c>
+      <c r="F60">
+        <v>0.32365414999999997</v>
+      </c>
+      <c r="G60">
+        <v>0.38526922000000002</v>
+      </c>
+      <c r="H60">
+        <v>0.72065780000000002</v>
+      </c>
+      <c r="I60">
+        <v>0.64802700000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>62</v>
       </c>
       <c r="B61">
-        <v>0.98582214000000001</v>
+        <v>0.61394375999999995</v>
       </c>
       <c r="C61">
-        <v>0.61671317000000003</v>
+        <v>0.97151200000000004</v>
       </c>
       <c r="D61">
-        <v>0.63034743000000004</v>
+        <v>0.73163307</v>
       </c>
       <c r="E61">
-        <v>0.69232309999999997</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.84027859999999999</v>
+      </c>
+      <c r="F61">
+        <v>0.31759733000000001</v>
+      </c>
+      <c r="G61">
+        <v>0.32429224000000001</v>
+      </c>
+      <c r="H61">
+        <v>0.88150110000000004</v>
+      </c>
+      <c r="I61">
+        <v>0.83681214000000004</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="2">
-        <v>0.52222222222222203</v>
+        <v>0.49166666666666597</v>
       </c>
       <c r="C62" s="2">
-        <v>0.51527777777777695</v>
+        <v>0.47638888888888797</v>
       </c>
       <c r="D62" s="2">
-        <v>0.83222222222222197</v>
+        <v>0.80777777777777704</v>
       </c>
       <c r="E62" s="2">
-        <v>0.82111111111111101</v>
+        <v>0.78888888888888897</v>
+      </c>
+      <c r="F62" s="2">
+        <v>0.70416666666666605</v>
+      </c>
+      <c r="G62" s="2">
+        <v>0.69722222222222197</v>
+      </c>
+      <c r="H62" s="2">
+        <v>0.81555555555555503</v>
+      </c>
+      <c r="I62" s="2">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64">
+        <v>0.62070000000000003</v>
+      </c>
+      <c r="C64">
+        <v>0.58620000000000005</v>
+      </c>
+      <c r="D64">
+        <v>0.7833</v>
+      </c>
+      <c r="E64">
+        <v>0.75</v>
+      </c>
+      <c r="F64">
+        <v>0.6552</v>
+      </c>
+      <c r="G64">
+        <v>0.70689999999999997</v>
+      </c>
+      <c r="H64">
+        <v>0.61670000000000003</v>
+      </c>
+      <c r="I64">
+        <v>0.66669999999999996</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65">
+        <v>0.22220000000000001</v>
+      </c>
+      <c r="C65">
+        <v>0.27779999999999999</v>
+      </c>
+      <c r="D65">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="E65">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="F65">
+        <v>0.1111</v>
+      </c>
+      <c r="G65">
+        <v>0.1111</v>
+      </c>
+      <c r="H65">
+        <v>0.9667</v>
+      </c>
+      <c r="I65">
+        <v>0.9667</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66">
+        <v>0.8</v>
+      </c>
+      <c r="C66">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D66">
+        <v>0.8</v>
+      </c>
+      <c r="E66">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="F66">
+        <v>0.9</v>
+      </c>
+      <c r="G66">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H66">
+        <v>0.26669999999999999</v>
+      </c>
+      <c r="I66">
+        <v>0.36670000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>